<commit_message>
cambios asociados a la asignacion de la concurrencia.
</commit_message>
<xml_diff>
--- a/bin/Debug/net6.0/movimientos_tarjeta.xlsx
+++ b/bin/Debug/net6.0/movimientos_tarjeta.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Tipo</t>
   </si>
@@ -21,6 +21,12 @@
   </si>
   <si>
     <t>Saldo Restante</t>
+  </si>
+  <si>
+    <t>Recarga</t>
+  </si>
+  <si>
+    <t>Consumo</t>
   </si>
 </sst>
 </file>
@@ -67,7 +73,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -84,6 +90,83 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0">
+        <v>200</v>
+      </c>
+      <c r="C2" s="0">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0">
+        <v>20</v>
+      </c>
+      <c r="C3" s="0">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0">
+        <v>500</v>
+      </c>
+      <c r="C4" s="0">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0">
+        <v>20</v>
+      </c>
+      <c r="C5" s="0">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="0">
+        <v>20</v>
+      </c>
+      <c r="C6" s="0">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="0">
+        <v>10</v>
+      </c>
+      <c r="C8" s="0">
+        <v>630</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>